<commit_message>
Prosseguimento do desenvolvimento da dissertação
</commit_message>
<xml_diff>
--- a/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/REVISAO_LITERATURA_ARTIGOS/Resumo_Autores_Descobertas.xlsx
+++ b/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/REVISAO_LITERATURA_ARTIGOS/Resumo_Autores_Descobertas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/2_ArtigosDesenvolvimentoMetodologia/pesquisa_20082019/REVISAO_LITERATURA_ARTIGOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1244940-D300-DC42-B025-C540F82AEEDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061196FA-1D0E-BB49-8164-37CA0611367D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="25320" windowHeight="15540" xr2:uid="{89A896A2-AE39-6E44-9686-4FFD0E9256A2}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -615,7 +614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD5D2C2-D2D9-174C-B12D-F2D8E2314A21}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="109" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="109" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>